<commit_message>
add the summary for yako axure 8
</commit_message>
<xml_diff>
--- a/featurelist.xlsx
+++ b/featurelist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14660" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="datagather" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>feature</t>
   </si>
@@ -113,6 +113,39 @@
   </si>
   <si>
     <t xml:space="preserve">  8.   add some feature survey to order out the list depending on the importance (AI, similar people radiar )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the  main page protype. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.  5th,May   Fred&amp;Yako  meeting minites </t>
+  </si>
+  <si>
+    <t>1.   using  Axure to draw the prototype</t>
+  </si>
+  <si>
+    <t>2.   common features(login, sign up, setting,...)   (owner: Fred Lei)</t>
+  </si>
+  <si>
+    <t>3.   main page:  (owner: Yako)</t>
+  </si>
+  <si>
+    <t>(top:  background (nice picture) and where to go function.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> next: Category by mood with small icon :  wedding, luxury,  sport, education, bar-life, peace</t>
+  </si>
+  <si>
+    <t>Next:  hot products list(nice picture with short words)  (can be clicked and jump to detail page)</t>
+  </si>
+  <si>
+    <t>Next:  customer blog (video, image, type of mood, address, time, (copy from douyin))</t>
+  </si>
+  <si>
+    <t>main function bars:   my Trips,  create trip, post blog, write review, me(setting)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> )</t>
   </si>
 </sst>
 </file>
@@ -535,10 +568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,6 +628,59 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>